<commit_message>
PREI y SAI con el gestor de archivos generado
</commit_message>
<xml_diff>
--- a/Implementación/PREI/2025_dates.xlsx
+++ b/Implementación/PREI/2025_dates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arman\Dropbox\3. Armando Cuaxospa\Reportes GPT 2025\mini_imss\Implementación\PREI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8F1132-AFC8-42BF-80EA-EA3EDDEACEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0267F93C-2AEA-427B-8FED-71F4C91771DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>DATE START</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>25/08/2025</t>
+  </si>
+  <si>
+    <t>01/01/2025</t>
+  </si>
+  <si>
+    <t>19/06/2025</t>
   </si>
 </sst>
 </file>
@@ -358,7 +364,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -367,7 +373,7 @@
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -380,9 +386,17 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>